<commit_message>
Beginning of code for intervention profits
</commit_message>
<xml_diff>
--- a/Data/Interventions.xlsx
+++ b/Data/Interventions.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Research\Practice Research\ERM\ERM154-Case Study Challenge\SRCSC 2024\Data\4FinalReview\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tmadf\Desktop\SOA2024\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CADDD202-8C5D-4906-850A-3D9D946B0C4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41887E08-F47B-4B76-A10D-5C27A6CD7AD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-40428" yWindow="-780" windowWidth="20376" windowHeight="12216" xr2:uid="{50D088CF-96A4-4C6D-BF14-DF418E47366A}"/>
+    <workbookView minimized="1" xWindow="30816" yWindow="4476" windowWidth="23040" windowHeight="12228" activeTab="1" xr2:uid="{50D088CF-96A4-4C6D-BF14-DF418E47366A}"/>
   </bookViews>
   <sheets>
     <sheet name="Interventions" sheetId="2" r:id="rId1"/>
+    <sheet name="Chosen Interventions" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="163">
   <si>
     <t xml:space="preserve"> Intervention Name                  </t>
   </si>
@@ -910,33 +911,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08A8FE2A-5E52-4EA3-89E7-6DCAEF06492E}">
   <dimension ref="A7:D67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="80.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.44140625" customWidth="1"/>
-    <col min="4" max="4" width="36.44140625" customWidth="1"/>
+    <col min="1" max="1" width="37.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="80.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.5" customWidth="1"/>
+    <col min="4" max="4" width="36.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
     </row>
-    <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>2024</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>160</v>
       </c>
       <c r="B11" s="6"/>
     </row>
-    <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>159</v>
       </c>
@@ -944,13 +945,13 @@
         <v>161</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="93" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>162</v>
       </c>
       <c r="B14" s="7"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>0</v>
       </c>
@@ -964,7 +965,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -978,7 +979,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -992,7 +993,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -1006,7 +1007,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -1020,7 +1021,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -1034,7 +1035,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -1048,7 +1049,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -1062,7 +1063,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1076,7 +1077,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1090,7 +1091,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -1104,7 +1105,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -1118,7 +1119,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -1132,7 +1133,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>37</v>
       </c>
@@ -1146,7 +1147,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>40</v>
       </c>
@@ -1160,7 +1161,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>43</v>
       </c>
@@ -1174,7 +1175,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>45</v>
       </c>
@@ -1188,7 +1189,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>48</v>
       </c>
@@ -1202,7 +1203,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>50</v>
       </c>
@@ -1216,7 +1217,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>52</v>
       </c>
@@ -1230,7 +1231,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>55</v>
       </c>
@@ -1244,7 +1245,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>58</v>
       </c>
@@ -1258,7 +1259,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>60</v>
       </c>
@@ -1272,7 +1273,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>62</v>
       </c>
@@ -1286,7 +1287,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>64</v>
       </c>
@@ -1300,7 +1301,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>66</v>
       </c>
@@ -1314,7 +1315,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>68</v>
       </c>
@@ -1328,7 +1329,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>70</v>
       </c>
@@ -1342,7 +1343,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>72</v>
       </c>
@@ -1356,7 +1357,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>75</v>
       </c>
@@ -1370,7 +1371,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>77</v>
       </c>
@@ -1384,7 +1385,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>79</v>
       </c>
@@ -1398,7 +1399,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>81</v>
       </c>
@@ -1412,7 +1413,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>83</v>
       </c>
@@ -1426,7 +1427,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>85</v>
       </c>
@@ -1440,7 +1441,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>87</v>
       </c>
@@ -1454,7 +1455,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>89</v>
       </c>
@@ -1468,7 +1469,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>91</v>
       </c>
@@ -1482,7 +1483,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>94</v>
       </c>
@@ -1496,7 +1497,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>96</v>
       </c>
@@ -1510,7 +1511,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>98</v>
       </c>
@@ -1524,7 +1525,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>100</v>
       </c>
@@ -1538,7 +1539,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>102</v>
       </c>
@@ -1552,7 +1553,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>104</v>
       </c>
@@ -1566,7 +1567,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>106</v>
       </c>
@@ -1580,7 +1581,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>108</v>
       </c>
@@ -1594,7 +1595,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>110</v>
       </c>
@@ -1608,7 +1609,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>112</v>
       </c>
@@ -1622,7 +1623,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>113</v>
       </c>
@@ -1636,7 +1637,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>114</v>
       </c>
@@ -1650,7 +1651,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>115</v>
       </c>
@@ -1672,4 +1673,123 @@
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3808A474-CE8E-4D83-A612-14C1DF8DDCAC}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="69.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>